<commit_message>
Remove unused code and update template
</commit_message>
<xml_diff>
--- a/public/assets/templates/update_assets.xlsx
+++ b/public/assets/templates/update_assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inventaris-lab\public\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7AF796-F3DE-42E9-8032-83F14F71D6D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87269FCA-5755-4867-ACE2-F9204276BFF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{312FC41A-3401-4073-B1A2-969A5FFE9C13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{312FC41A-3401-4073-B1A2-969A5FFE9C13}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_ruangan" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>processor</t>
-  </si>
-  <si>
-    <t>os</t>
   </si>
   <si>
     <t>memory</t>
@@ -193,6 +190,15 @@
   </si>
   <si>
     <t>KODE aset merupakan 4 digit random yang terdiri atas A-Z,a-z,0-9 (jika dikosongkan akan digenerate oleh sistem secara otomatis)</t>
+  </si>
+  <si>
+    <t>os1</t>
+  </si>
+  <si>
+    <t>os2</t>
+  </si>
+  <si>
+    <t>os3</t>
   </si>
 </sst>
 </file>
@@ -593,19 +599,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,17 +658,17 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -709,23 +715,23 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -738,20 +744,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20AC27E-EB95-425A-B3FD-88D8A6B82BCC}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -762,8 +768,10 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -777,34 +785,40 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -814,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E81C86E-B713-40A0-908B-2CA99AFF8E84}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
@@ -883,50 +897,50 @@
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>